<commit_message>
add NEW SHEETS and veba excel olusturma
</commit_message>
<xml_diff>
--- a/sheets/DISAR - FEDERICO GRAVINA - ISTANBULUN ANLATIMI - Karaoglan.xlsx
+++ b/sheets/DISAR - FEDERICO GRAVINA - ISTANBULUN ANLATIMI - Karaoglan.xlsx
@@ -298,7 +298,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -371,7 +371,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +382,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4F81BD"/>
         <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7B3CA"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -426,23 +432,31 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -475,7 +489,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -504,7 +530,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB7B3CA"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -559,15 +585,15 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="135.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="16.29"/>
@@ -576,298 +602,298 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="2" width="8.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="8" customFormat="true" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="11" t="n">
         <v>26</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="9" t="n">
+      <c r="H2" s="11" t="n">
         <v>2008</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="11" t="n">
         <v>35</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="9" t="n">
+      <c r="H3" s="11" t="n">
         <v>2008</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="11" t="n">
         <v>36</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="9" t="n">
+      <c r="H4" s="11" t="n">
         <v>2008</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="9" t="n">
+      <c r="D5" s="11" t="n">
         <v>36</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="9" t="n">
+      <c r="H5" s="11" t="n">
         <v>2008</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="11" t="n">
         <v>37</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="9" t="n">
+      <c r="H6" s="11" t="n">
         <v>2008</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="11" t="n">
         <v>38</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="9" t="n">
+      <c r="H7" s="11" t="n">
         <v>2008</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="9" t="n">
+      <c r="D8" s="11" t="n">
         <v>69</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="9" t="n">
+      <c r="H8" s="11" t="n">
         <v>2008</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="11" t="n">
         <v>69</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="9" t="n">
+      <c r="H9" s="11" t="n">
         <v>2008</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="9" t="n">
+      <c r="D10" s="11" t="n">
         <v>69</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="9" t="n">
+      <c r="H10" s="11" t="n">
         <v>2008</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="0"/>
       <c r="C11" s="0"/>
       <c r="D11" s="0"/>
@@ -882,7 +908,7 @@
       <c r="M11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="0"/>
       <c r="C12" s="0"/>
       <c r="D12" s="0"/>
@@ -897,7 +923,7 @@
       <c r="M12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="0"/>
       <c r="C13" s="0"/>
       <c r="D13" s="0"/>
@@ -912,7 +938,7 @@
       <c r="M13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="0"/>
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
@@ -927,7 +953,7 @@
       <c r="M14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="0"/>
       <c r="C15" s="0"/>
       <c r="D15" s="0"/>
@@ -942,7 +968,7 @@
       <c r="M15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
       <c r="D16" s="0"/>
@@ -957,7 +983,7 @@
       <c r="M16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="0"/>
       <c r="C17" s="0"/>
       <c r="D17" s="0"/>
@@ -972,7 +998,7 @@
       <c r="M17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
       <c r="D18" s="0"/>
@@ -987,7 +1013,7 @@
       <c r="M18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="0"/>
       <c r="C19" s="0"/>
       <c r="D19" s="0"/>
@@ -1002,7 +1028,7 @@
       <c r="M19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="0"/>
       <c r="C20" s="0"/>
       <c r="D20" s="0"/>
@@ -1017,7 +1043,7 @@
       <c r="M20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
       <c r="D21" s="0"/>
@@ -1032,7 +1058,7 @@
       <c r="M21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="0"/>
       <c r="C22" s="0"/>
       <c r="D22" s="0"/>
@@ -1047,7 +1073,7 @@
       <c r="M22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
       <c r="D23" s="0"/>
@@ -1062,7 +1088,7 @@
       <c r="M23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="0"/>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
@@ -1077,7 +1103,7 @@
       <c r="M24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="0"/>
       <c r="C25" s="0"/>
       <c r="D25" s="0"/>
@@ -1092,7 +1118,7 @@
       <c r="M25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="0"/>
       <c r="C26" s="0"/>
       <c r="D26" s="0"/>
@@ -1107,7 +1133,7 @@
       <c r="M26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="0"/>
       <c r="C27" s="0"/>
       <c r="D27" s="0"/>
@@ -1122,7 +1148,7 @@
       <c r="M27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="0"/>
       <c r="C28" s="0"/>
       <c r="D28" s="0"/>

</xml_diff>